<commit_message>
Hämta poster (sida) och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsplan.xlsx
+++ b/dokumentation/Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60915\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11077A56-FFA1-4F0A-9A57-D1A06D07336E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF517C-7114-4E66-AC5D-CE8EB97B545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{377EFEFC-62B7-4081-9E2C-D9EAF734AD18}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Uppgift</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Uppdatera aktivitet + Test</t>
+  </si>
+  <si>
+    <t>Radera aktivitet + Test</t>
   </si>
 </sst>
 </file>
@@ -314,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C19" totalsRowShown="0">
-  <autoFilter ref="A1:C19" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CDBCB945-AC94-456B-932C-F3FE5625D63E}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{1C9B714A-84F6-4B14-B81D-D97D8B8F84F5}" name="Antal lektioner"/>
@@ -976,10 +979,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C51A9B-A327-4960-BD6C-0FC18D23BC20}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,10 +1192,21 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8">
+        <v>45314</v>
+      </c>
+      <c r="B19">
+        <v>1.5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B20" s="9">
         <f>SUBTOTAL(109,B2:B18)</f>
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Tester för spara uppgift funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsplan.xlsx
+++ b/dokumentation/Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60915\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF517C-7114-4E66-AC5D-CE8EB97B545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863BE0B-941B-4942-88D7-9EAE85EAA865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{377EFEFC-62B7-4081-9E2C-D9EAF734AD18}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Uppgift</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Radera aktivitet + Test</t>
+  </si>
+  <si>
+    <t>Hämta uppgifter med sida + Test</t>
+  </si>
+  <si>
+    <t>Hämta uppgifter med datum + Test</t>
   </si>
 </sst>
 </file>
@@ -317,8 +323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C20" totalsRowShown="0">
-  <autoFilter ref="A1:C20" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CDBCB945-AC94-456B-932C-F3FE5625D63E}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{1C9B714A-84F6-4B14-B81D-D97D8B8F84F5}" name="Antal lektioner"/>
@@ -979,17 +985,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C51A9B-A327-4960-BD6C-0FC18D23BC20}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1203,12 +1209,34 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8">
+        <v>45314</v>
+      </c>
+      <c r="B20">
+        <v>2.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>45315</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="9">
-        <f>SUBTOTAL(109,B2:B18)</f>
-        <v>32</v>
+      <c r="B22" s="9">
+        <f>SUBTOTAL(109,B2:B21)</f>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hämta enskild uppgift och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsplan.xlsx
+++ b/dokumentation/Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60915\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F863BE0B-941B-4942-88D7-9EAE85EAA865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DAE42-A5CC-44A6-987A-6A02B864528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{377EFEFC-62B7-4081-9E2C-D9EAF734AD18}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Uppgift</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t>Hämta uppgifter med datum + Test</t>
+  </si>
+  <si>
+    <t>Spara ny post tester</t>
+  </si>
+  <si>
+    <t>Kontrollera indata tester</t>
+  </si>
+  <si>
+    <t>Hämta enskild uppgift + Test</t>
   </si>
 </sst>
 </file>
@@ -323,8 +332,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C22" totalsRowShown="0">
-  <autoFilter ref="A1:C22" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C25" totalsRowShown="0">
+  <autoFilter ref="A1:C25" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CDBCB945-AC94-456B-932C-F3FE5625D63E}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{1C9B714A-84F6-4B14-B81D-D97D8B8F84F5}" name="Antal lektioner"/>
@@ -985,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C51A9B-A327-4960-BD6C-0FC18D23BC20}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,12 +1240,45 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8">
+        <v>45317</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>45317</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>45317</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="9">
-        <f>SUBTOTAL(109,B2:B21)</f>
-        <v>38</v>
+      <c r="B25" s="9">
+        <f>SUBTOTAL(109,B2:B23)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uppdatera uppgift och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsplan.xlsx
+++ b/dokumentation/Tidsplan.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60915\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DAE42-A5CC-44A6-987A-6A02B864528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DDD541-F91D-48CA-AAFE-9F39723A4152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{377EFEFC-62B7-4081-9E2C-D9EAF734AD18}"/>
   </bookViews>
@@ -1277,8 +1277,8 @@
         <v>31</v>
       </c>
       <c r="B25" s="9">
-        <f>SUBTOTAL(109,B2:B23)</f>
-        <v>40</v>
+        <f>SUBTOTAL(109,B2:B24)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compilation och tester funkar
</commit_message>
<xml_diff>
--- a/dokumentation/Tidsplan.xlsx
+++ b/dokumentation/Tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\~60915\tidsredovisning\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DDD541-F91D-48CA-AAFE-9F39723A4152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFE796E-418A-4195-B399-69D7B508691E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{377EFEFC-62B7-4081-9E2C-D9EAF734AD18}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Uppgift</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>Hämta enskild uppgift + Test</t>
+  </si>
+  <si>
+    <t>Uppdatera uppgift + Test</t>
+  </si>
+  <si>
+    <t>Radera uppgift + Test</t>
+  </si>
+  <si>
+    <t>Hämta tidsvy + Test</t>
   </si>
 </sst>
 </file>
@@ -332,8 +341,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C25" totalsRowShown="0">
-  <autoFilter ref="A1:C25" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}" name="Tabell2" displayName="Tabell2" ref="A1:C28" totalsRowShown="0">
+  <autoFilter ref="A1:C28" xr:uid="{45F3BAF2-B181-4664-8A40-F28E492F35BA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CDBCB945-AC94-456B-932C-F3FE5625D63E}" name="Datum"/>
     <tableColumn id="2" xr3:uid="{1C9B714A-84F6-4B14-B81D-D97D8B8F84F5}" name="Antal lektioner"/>
@@ -994,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C51A9B-A327-4960-BD6C-0FC18D23BC20}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,12 +1282,45 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8">
+        <v>45320</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>45320</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>45322</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="9">
-        <f>SUBTOTAL(109,B2:B24)</f>
-        <v>42</v>
+      <c r="B28" s="9">
+        <f>SUBTOTAL(109,B2:B26)</f>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>